<commit_message>
updating cigna healthguard benefits
</commit_message>
<xml_diff>
--- a/Inputs/Cigna/info.xlsx
+++ b/Inputs/Cigna/info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">provider</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">frequencyFrom</t>
   </si>
   <si>
+    <t xml:space="preserve">addons</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cigna</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dental/Maternity (Consultations, Scans and Delivery)/Optical Benefits/Wellness &amp; Health Screening</t>
   </si>
 </sst>
 </file>
@@ -168,13 +174,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.42"/>
@@ -205,13 +211,16 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>3.6745</v>
@@ -223,13 +232,16 @@
         <v>45657</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>